<commit_message>
updated to run in local
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D38681-FB6F-4AA1-9030-D6AF782D9FB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
   <si>
     <t>testname</t>
   </si>
@@ -117,12 +118,15 @@
   </si>
   <si>
     <t>69.0</t>
+  </si>
+  <si>
+    <t>90.0.4430.93</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -257,6 +261,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -292,6 +313,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,23 +505,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="101.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -517,7 +555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -534,7 +572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -558,25 +596,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" customWidth="1"/>
-    <col min="2" max="3" width="18.08984375" customWidth="1"/>
-    <col min="4" max="4" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6328125" customWidth="1"/>
-    <col min="6" max="6" width="29.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="40.5546875" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,18 +640,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>15</v>
@@ -628,7 +666,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -654,12 +692,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
@@ -680,7 +718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -706,12 +744,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>23</v>
@@ -732,7 +770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -758,7 +796,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -784,7 +822,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:8" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -812,5 +850,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>